<commit_message>
Added entry in activity log
</commit_message>
<xml_diff>
--- a/jaclemon.xlsx
+++ b/jaclemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorda\306PRE_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12302E0C-95A6-47B9-8DF0-D30982A476A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E3EDD3-03B0-4A96-BE02-CECFB6FA0F74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>DATE</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Setting up Github repo for project</t>
+  </si>
+  <si>
+    <t>Created function to allow program to intake command line arguments using C on notepad++</t>
   </si>
 </sst>
 </file>
@@ -364,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,6 +407,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43864</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added entry to activity log
</commit_message>
<xml_diff>
--- a/jaclemon.xlsx
+++ b/jaclemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorda\306PRE_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656BA3CB-EBC4-4BCB-AB77-545613A420C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EA90C1-7415-42E7-A479-F3718C8C0102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     <t>Created function to allow program to intake command line arguments using C on notepad++</t>
   </si>
   <si>
-    <t>60 minutess</t>
+    <t>60 minutesss</t>
   </si>
 </sst>
 </file>

</xml_diff>